<commit_message>
added test case for slider storage added test cases for autostart model and REST interface
</commit_message>
<xml_diff>
--- a/Tests/integrationTests/01b_ARE startup/Test_cases_ARE_startup.xlsx
+++ b/Tests/integrationTests/01b_ARE startup/Test_cases_ARE_startup.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Number</t>
   </si>
@@ -245,6 +245,63 @@
 3. DO NOT plug in Gamepad
 4.Execute ARE start file
 5. Restore original model file</t>
+  </si>
+  <si>
+    <t>Define autostart model per command line parameter</t>
+  </si>
+  <si>
+    <t>TestModelAutostart.acs
+ARE start file: start.bat (start.sh - Linux, Mac OS X)
+Command shell: cmd.exe (xterm or similar - Linux, Mac OS X)</t>
+  </si>
+  <si>
+    <t>The ARE must start successfully and the model 'TestModelAutostart.acs' must be started automatically</t>
+  </si>
+  <si>
+    <t>Start ARE without webservice</t>
+  </si>
+  <si>
+    <t>1. The page must not be loadable (err_connection_refused)
+2. The page must not be loadable (err_connection_refused)</t>
+  </si>
+  <si>
+    <t>Start ARE with webservice</t>
+  </si>
+  <si>
+    <t>1. The page must be loadable and stating 'CONNECTED'  to the websocket
+2. The page must be loadable and return the currently deployed model in xml</t>
+  </si>
+  <si>
+    <t>ARE_START_7</t>
+  </si>
+  <si>
+    <t>ARE_START_8</t>
+  </si>
+  <si>
+    <t>ARE_START_9</t>
+  </si>
+  <si>
+    <t>0. Copy model to bin/ARE/models
+1. Open command shell in bin/ARE directory
+2. Execute 
+start.bat TestModelAutostart.acs
+./start.sh TestModelAutostart.acs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0. Copy model to bin/ARE/models
+1. Open http://localhost:8082/
+2. Open http://localhost:8081/rest/runtime/model
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0. Copy model to bin/ARE/models
+1. Open command shell in bin/ARE directory
+2. Execute 
+start.bat --webservice TestModelAutostart.acs
+./start.sh --webservice TestModelAutostart.acs
+3. Open http://localhost:8082/
+4. Open http://localhost:8081/rest/runtime/model
+</t>
   </si>
 </sst>
 </file>
@@ -623,7 +680,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -633,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -811,27 +868,57 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="A13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="120.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="A14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="A15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>